<commit_message>
Made changes to lab2
</commit_message>
<xml_diff>
--- a/Visualization/Assignment_2/baseball-2016.xlsx
+++ b/Visualization/Assignment_2/baseball-2016.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C3F3E8-634B-497B-9C34-0E4BA1DE3085}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A1C3F3E8-634B-497B-9C34-0E4BA1DE3085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8DB4EC75-1BB7-4549-B53F-5D87888FA16A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="14028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,17 +519,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34:K35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +615,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -701,7 +701,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -787,7 +787,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -873,7 +873,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -959,7 +959,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>59</v>
       </c>

</xml_diff>